<commit_message>
Modified the summer to do list
</commit_message>
<xml_diff>
--- a/Workplan/SummerToDo.xlsx
+++ b/Workplan/SummerToDo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Include Fio's part (https://michelilab.stanford.edu/micheli)</t>
   </si>
@@ -99,7 +99,31 @@
     <t>Modify R package to include new functions for new indicators, and allso for more flexibility</t>
   </si>
   <si>
-    <t>Vignette of R package</t>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>July 2nd</t>
+  </si>
+  <si>
+    <t>June 26</t>
+  </si>
+  <si>
+    <t>July 6</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>All summer long!</t>
+  </si>
+  <si>
+    <t>June 28</t>
+  </si>
+  <si>
+    <t>July 1st</t>
+  </si>
+  <si>
+    <t>Update Vignette of R package</t>
   </si>
 </sst>
 </file>
@@ -431,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -443,15 +467,18 @@
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -459,23 +486,29 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -483,39 +516,51 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -523,7 +568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -531,7 +576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -539,7 +584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -547,39 +592,51 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>5</v>
       </c>

</xml_diff>